<commit_message>
Acrescenta estimativas de todos os primeiros 5 indicadores utilizados no MVP, corrige falhas pontuais e acrescenta script main/do
</commit_message>
<xml_diff>
--- a/outputs/mvp/ind_1_1_1/ind_1_1_1.xlsx
+++ b/outputs/mvp/ind_1_1_1/ind_1_1_1.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,17 +417,17 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.1067173865411062</v>
+        <v>0.1077555284150259</v>
       </c>
       <c r="C3">
-        <v>0.1041888192307831</v>
+        <v>0.1052346496721633</v>
       </c>
       <c r="D3">
-        <v>0.1092459538514293</v>
+        <v>0.1102764071578885</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
     </row>
@@ -438,22 +438,17 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.04922019959981231</v>
+        <v>0.1067173865411062</v>
       </c>
       <c r="C4">
-        <v>0.02047016498604594</v>
+        <v>0.1041888192307831</v>
       </c>
       <c r="D4">
-        <v>0.07797023421357868</v>
+        <v>0.1092459538514293</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>Masculino</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Amarela</t>
         </is>
       </c>
     </row>
@@ -464,22 +459,22 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.05860772739432404</v>
+        <v>0.03836442158217402</v>
       </c>
       <c r="C5">
-        <v>0.05615703691342971</v>
+        <v>0.01923234229945393</v>
       </c>
       <c r="D5">
-        <v>0.06105841787521837</v>
+        <v>0.05749650086489411</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Amarela</t>
         </is>
       </c>
     </row>
@@ -490,13 +485,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.04922019959981231</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.02047016498604594</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.07797023421357868</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -505,7 +500,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Ignorado</t>
+          <t>Amarela</t>
         </is>
       </c>
     </row>
@@ -516,22 +511,22 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.2056090128440956</v>
+        <v>0.05719558779292232</v>
       </c>
       <c r="C7">
-        <v>0.1412154026158309</v>
+        <v>0.0545962583504882</v>
       </c>
       <c r="D7">
-        <v>0.2700026230723603</v>
+        <v>0.05979491723535645</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Branca</t>
         </is>
       </c>
     </row>
@@ -542,13 +537,13 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.1455411125169712</v>
+        <v>0.05860772739432404</v>
       </c>
       <c r="C8">
-        <v>0.141489102453384</v>
+        <v>0.05615703691342971</v>
       </c>
       <c r="D8">
-        <v>0.1495931225805584</v>
+        <v>0.06105841787521837</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -557,7 +552,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Branca</t>
         </is>
       </c>
     </row>
@@ -568,27 +563,22 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.0395175403864721</v>
+        <v>0.547942177629459</v>
       </c>
       <c r="C9">
-        <v>0.009159216176208244</v>
+        <v>-0.05354854053967262</v>
       </c>
       <c r="D9">
-        <v>0.06987586459673596</v>
+        <v>1.14943289579859</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Amarela</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Ignorado</t>
         </is>
       </c>
     </row>
@@ -599,13 +589,13 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.04361804634938695</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0.04104223264545248</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0.04619386005332142</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -614,12 +604,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Ignorado</t>
         </is>
       </c>
     </row>
@@ -630,27 +615,22 @@
         </is>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0.1690496088382455</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.112277010422408</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.2258222072540829</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Ignorado</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Indígena</t>
         </is>
       </c>
     </row>
@@ -661,13 +641,13 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.1681675975568784</v>
+        <v>0.2056090128440956</v>
       </c>
       <c r="C12">
-        <v>0.09693889576422837</v>
+        <v>0.1412154026158309</v>
       </c>
       <c r="D12">
-        <v>0.2393962993495284</v>
+        <v>0.2700026230723603</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -677,11 +657,6 @@
       <c r="F12" t="inlineStr">
         <is>
           <t>Indígena</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -692,27 +667,22 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.1044096138081008</v>
+        <v>0.1520285941557457</v>
       </c>
       <c r="C13">
-        <v>0.1000724231128585</v>
+        <v>0.1480190680868821</v>
       </c>
       <c r="D13">
-        <v>0.1087468045033431</v>
+        <v>0.1560381202246092</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>Preto ou pardo</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -723,13 +693,13 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.2064841774806512</v>
+        <v>0.1455411125169712</v>
       </c>
       <c r="C14">
-        <v>0.08366085869726865</v>
+        <v>0.141489102453384</v>
       </c>
       <c r="D14">
-        <v>0.3293074962640338</v>
+        <v>0.1495931225805584</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -738,12 +708,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Amarela</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
     </row>
@@ -754,27 +719,27 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.1693578553493132</v>
+        <v>0.03414687468430796</v>
       </c>
       <c r="C15">
-        <v>0.1585350259976693</v>
+        <v>0.01442365872164525</v>
       </c>
       <c r="D15">
-        <v>0.1801806847009571</v>
+        <v>0.05387009064697067</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -785,13 +750,13 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.3843262963645647</v>
+        <v>0.0395175403864721</v>
       </c>
       <c r="C16">
-        <v>0.2449107313705934</v>
+        <v>0.009159216176208244</v>
       </c>
       <c r="D16">
-        <v>0.5237418613585361</v>
+        <v>0.06987586459673596</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -800,12 +765,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -816,102 +781,137 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.3201489087125678</v>
+        <v>0.0429929756238225</v>
       </c>
       <c r="C17">
-        <v>0.3107084358507918</v>
+        <v>0.0402810519915398</v>
       </c>
       <c r="D17">
-        <v>0.3295893815743438</v>
+        <v>0.04570489925610521</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B18">
-        <v>0.06924122814792455</v>
+        <v>0.04361804634938695</v>
       </c>
       <c r="C18">
-        <v>0.06700591338730398</v>
+        <v>0.04104223264545248</v>
       </c>
       <c r="D18">
-        <v>0.07147654290854512</v>
+        <v>0.04619386005332142</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B19">
-        <v>0.06969957259703537</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>0.06736003505919752</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0.07203911013487321</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
           <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B20">
-        <v>0.06876192800282943</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>0.06636935892646212</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0.07115449707919674</v>
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
           <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B21">
-        <v>0.05690056744754991</v>
+        <v>0.1269812982491658</v>
       </c>
       <c r="C21">
-        <v>0.04000406267686278</v>
+        <v>0.06822599463120882</v>
       </c>
       <c r="D21">
-        <v>0.07379707221823704</v>
+        <v>0.1857366018671228</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -920,24 +920,29 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B22">
-        <v>0.0630473992577661</v>
+        <v>0.1681675975568784</v>
       </c>
       <c r="C22">
-        <v>0.03570223759902014</v>
+        <v>0.09693889576422837</v>
       </c>
       <c r="D22">
-        <v>0.09039256091651207</v>
+        <v>0.2393962993495284</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -946,24 +951,29 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B23">
-        <v>0.040116023202247</v>
+        <v>0.1141770562689356</v>
       </c>
       <c r="C23">
-        <v>0.03789355035290268</v>
+        <v>0.1096386265718891</v>
       </c>
       <c r="D23">
-        <v>0.04233849605159132</v>
+        <v>0.1187154859659822</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -972,24 +982,29 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B24">
-        <v>0.03952726715739519</v>
+        <v>0.1044096138081008</v>
       </c>
       <c r="C24">
-        <v>0.03721841441200474</v>
+        <v>0.1000724231128585</v>
       </c>
       <c r="D24">
-        <v>0.04183611990278564</v>
+        <v>0.1087468045033431</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -998,24 +1013,29 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B25">
-        <v>0.04397793649124208</v>
+        <v>0.1217234321957831</v>
       </c>
       <c r="C25">
-        <v>-0.02727489791412698</v>
+        <v>0.04817577606463851</v>
       </c>
       <c r="D25">
-        <v>0.1152307708966111</v>
+        <v>0.1952710883269278</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1024,24 +1044,29 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Ignorado</t>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B26">
-        <v>0.1288491536471042</v>
+        <v>0.2064841774806512</v>
       </c>
       <c r="C26">
-        <v>-0.04901483159892142</v>
+        <v>0.08366085869726865</v>
       </c>
       <c r="D26">
-        <v>0.3067131388931298</v>
+        <v>0.3293074962640338</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1050,24 +1075,29 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Ignorado</t>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B27">
-        <v>0.09077607592597677</v>
+        <v>0.1786886683493295</v>
       </c>
       <c r="C27">
-        <v>0.06614113963765586</v>
+        <v>0.166166435152406</v>
       </c>
       <c r="D27">
-        <v>0.1154110122142977</v>
+        <v>0.191210901546253</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1076,24 +1106,29 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B28">
-        <v>0.08603253087970009</v>
+        <v>0.1693578553493132</v>
       </c>
       <c r="C28">
-        <v>0.06052607930385365</v>
+        <v>0.1585350259976693</v>
       </c>
       <c r="D28">
-        <v>0.1115389824555465</v>
+        <v>0.1801806847009571</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1102,24 +1137,29 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B29">
-        <v>0.09289066147244007</v>
+        <v>0.3898343053661995</v>
       </c>
       <c r="C29">
-        <v>0.08933422823958206</v>
+        <v>-0.2954529790628765</v>
       </c>
       <c r="D29">
-        <v>0.09644709470529808</v>
+        <v>1.075121589795276</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1128,126 +1168,136 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B30">
-        <v>0.09052670600977686</v>
+        <v>0.3641963620849838</v>
       </c>
       <c r="C30">
-        <v>0.08722282219865291</v>
+        <v>0.2206456189526247</v>
       </c>
       <c r="D30">
-        <v>0.09383058982090081</v>
+        <v>0.507747105217343</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B31">
-        <v>0.05337295832516659</v>
+        <v>0.3843262963645647</v>
       </c>
       <c r="C31">
-        <v>0.03519586192159806</v>
+        <v>0.2449107313705934</v>
       </c>
       <c r="D31">
-        <v>0.07155005472873513</v>
+        <v>0.5237418613585361</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B32">
-        <v>0.04906234186894141</v>
+        <v>0.3367118684632939</v>
       </c>
       <c r="C32">
-        <v>0.01906166929770911</v>
+        <v>0.3268788949605854</v>
       </c>
       <c r="D32">
-        <v>0.0790630144401737</v>
+        <v>0.3465448419660024</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B33">
-        <v>0.03247678207038816</v>
+        <v>0.3201489087125678</v>
       </c>
       <c r="C33">
-        <v>0.0302513465389829</v>
+        <v>0.3107084358507918</v>
       </c>
       <c r="D33">
-        <v>0.03470221760179343</v>
+        <v>0.3295893815743438</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
@@ -1258,28 +1308,13 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.03104802298978394</v>
+        <v>0.06924122814792455</v>
       </c>
       <c r="C34">
-        <v>0.02876501123393008</v>
+        <v>0.06700591338730398</v>
       </c>
       <c r="D34">
-        <v>0.03333103474563781</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Urbana</t>
-        </is>
+        <v>0.07147654290854512</v>
       </c>
     </row>
     <row r="35">
@@ -1289,27 +1324,17 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.04409003357927133</v>
+        <v>0.06969957259703537</v>
       </c>
       <c r="C35">
-        <v>-0.02740207776296817</v>
+        <v>0.06736003505919752</v>
       </c>
       <c r="D35">
-        <v>0.1155821449215108</v>
+        <v>0.07203911013487321</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
           <t>Feminino</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Ignorado</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -1320,27 +1345,17 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.1309669316087286</v>
+        <v>0.06876192800282943</v>
       </c>
       <c r="C36">
-        <v>-0.04965823300381697</v>
+        <v>0.06636935892646212</v>
       </c>
       <c r="D36">
-        <v>0.3115920962212742</v>
+        <v>0.07115449707919674</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
           <t>Masculino</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Ignorado</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -1351,13 +1366,13 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.07000629753765267</v>
+        <v>0.05690056744754991</v>
       </c>
       <c r="C37">
-        <v>0.04284481472592563</v>
+        <v>0.04000406267686278</v>
       </c>
       <c r="D37">
-        <v>0.0971677803493797</v>
+        <v>0.07379707221823704</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1366,12 +1381,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Indígena</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Amarela</t>
         </is>
       </c>
     </row>
@@ -1382,13 +1392,13 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.05942416420103389</v>
+        <v>0.0630473992577661</v>
       </c>
       <c r="C38">
-        <v>0.03182497350489777</v>
+        <v>0.03570223759902014</v>
       </c>
       <c r="D38">
-        <v>0.08702335489717</v>
+        <v>0.09039256091651207</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1397,12 +1407,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Indígena</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Amarela</t>
         </is>
       </c>
     </row>
@@ -1413,13 +1418,13 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.07286359808387763</v>
+        <v>0.040116023202247</v>
       </c>
       <c r="C39">
-        <v>0.06942407948457623</v>
+        <v>0.03789355035290268</v>
       </c>
       <c r="D39">
-        <v>0.07630311668317903</v>
+        <v>0.04233849605159132</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1428,12 +1433,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Branca</t>
         </is>
       </c>
     </row>
@@ -1444,13 +1444,13 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.06860137834941644</v>
+        <v>0.03952726715739519</v>
       </c>
       <c r="C40">
-        <v>0.06528994464618545</v>
+        <v>0.03721841441200474</v>
       </c>
       <c r="D40">
-        <v>0.07191281205264743</v>
+        <v>0.04183611990278564</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1459,12 +1459,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Branca</t>
         </is>
       </c>
     </row>
@@ -1475,13 +1470,13 @@
         </is>
       </c>
       <c r="B41">
-        <v>0.09380635946879537</v>
+        <v>0.04397793649124208</v>
       </c>
       <c r="C41">
-        <v>0.04549894925610921</v>
+        <v>-0.02727489791412698</v>
       </c>
       <c r="D41">
-        <v>0.1421137696814815</v>
+        <v>0.1152307708966111</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1490,12 +1485,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Amarela</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Ignorado</t>
         </is>
       </c>
     </row>
@@ -1506,13 +1496,13 @@
         </is>
       </c>
       <c r="B42">
-        <v>0.1739309196846933</v>
+        <v>0.1288491536471042</v>
       </c>
       <c r="C42">
-        <v>0.1188232112976242</v>
+        <v>-0.04901483159892142</v>
       </c>
       <c r="D42">
-        <v>0.2290386280717624</v>
+        <v>0.3067131388931298</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1521,12 +1511,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Amarela</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Ignorado</t>
         </is>
       </c>
     </row>
@@ -1537,13 +1522,13 @@
         </is>
       </c>
       <c r="B43">
-        <v>0.1115463158419633</v>
+        <v>0.09077607592597677</v>
       </c>
       <c r="C43">
-        <v>0.1015179294887903</v>
+        <v>0.06614113963765586</v>
       </c>
       <c r="D43">
-        <v>0.1215747021951363</v>
+        <v>0.1154110122142977</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1552,12 +1537,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Indígena</t>
         </is>
       </c>
     </row>
@@ -1568,13 +1548,13 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.106629481332095</v>
+        <v>0.08603253087970009</v>
       </c>
       <c r="C44">
-        <v>0.09765589680271874</v>
+        <v>0.06052607930385365</v>
       </c>
       <c r="D44">
-        <v>0.1156030658614713</v>
+        <v>0.1115389824555465</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1583,12 +1563,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Indígena</t>
         </is>
       </c>
     </row>
@@ -1599,13 +1574,13 @@
         </is>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>0.09289066147244007</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>0.08933422823958206</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>0.09644709470529808</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1614,12 +1589,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Ignorado</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
     </row>
@@ -1630,13 +1600,13 @@
         </is>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>0.09052670600977686</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>0.08722282219865291</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>0.09383058982090081</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1645,12 +1615,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Ignorado</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
     </row>
@@ -1661,13 +1626,13 @@
         </is>
       </c>
       <c r="B47">
-        <v>0.2058788810495588</v>
+        <v>0.05337295832516659</v>
       </c>
       <c r="C47">
-        <v>0.134474776128396</v>
+        <v>0.03519586192159806</v>
       </c>
       <c r="D47">
-        <v>0.2772829859707216</v>
+        <v>0.07155005472873513</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1676,12 +1641,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -1692,13 +1657,13 @@
         </is>
       </c>
       <c r="B48">
-        <v>0.1986631874191323</v>
+        <v>0.04906234186894141</v>
       </c>
       <c r="C48">
-        <v>0.1310071918645423</v>
+        <v>0.01906166929770911</v>
       </c>
       <c r="D48">
-        <v>0.2663191829737223</v>
+        <v>0.0790630144401737</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1707,12 +1672,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -1723,13 +1688,13 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.2089163878490449</v>
+        <v>0.03247678207038816</v>
       </c>
       <c r="C49">
-        <v>0.1974025289192148</v>
+        <v>0.0302513465389829</v>
       </c>
       <c r="D49">
-        <v>0.2204302467788751</v>
+        <v>0.03470221760179343</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1738,12 +1703,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -1754,25 +1719,521 @@
         </is>
       </c>
       <c r="B50">
+        <v>0.03104802298978394</v>
+      </c>
+      <c r="C50">
+        <v>0.02876501123393008</v>
+      </c>
+      <c r="D50">
+        <v>0.03333103474563781</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B51">
+        <v>0.04409003357927133</v>
+      </c>
+      <c r="C51">
+        <v>-0.02740207776296817</v>
+      </c>
+      <c r="D51">
+        <v>0.1155821449215108</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B52">
+        <v>0.1309669316087286</v>
+      </c>
+      <c r="C52">
+        <v>-0.04965823300381697</v>
+      </c>
+      <c r="D52">
+        <v>0.3115920962212742</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B53">
+        <v>0.07000629753765267</v>
+      </c>
+      <c r="C53">
+        <v>0.04284481472592563</v>
+      </c>
+      <c r="D53">
+        <v>0.0971677803493797</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B54">
+        <v>0.05942416420103389</v>
+      </c>
+      <c r="C54">
+        <v>0.03182497350489777</v>
+      </c>
+      <c r="D54">
+        <v>0.08702335489717</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B55">
+        <v>0.07286359808387763</v>
+      </c>
+      <c r="C55">
+        <v>0.06942407948457623</v>
+      </c>
+      <c r="D55">
+        <v>0.07630311668317903</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B56">
+        <v>0.06860137834941644</v>
+      </c>
+      <c r="C56">
+        <v>0.06528994464618545</v>
+      </c>
+      <c r="D56">
+        <v>0.07191281205264743</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B57">
+        <v>0.09380635946879537</v>
+      </c>
+      <c r="C57">
+        <v>0.04549894925610921</v>
+      </c>
+      <c r="D57">
+        <v>0.1421137696814815</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B58">
+        <v>0.1739309196846933</v>
+      </c>
+      <c r="C58">
+        <v>0.1188232112976242</v>
+      </c>
+      <c r="D58">
+        <v>0.2290386280717624</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B59">
+        <v>0.1115463158419633</v>
+      </c>
+      <c r="C59">
+        <v>0.1015179294887903</v>
+      </c>
+      <c r="D59">
+        <v>0.1215747021951363</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B60">
+        <v>0.106629481332095</v>
+      </c>
+      <c r="C60">
+        <v>0.09765589680271874</v>
+      </c>
+      <c r="D60">
+        <v>0.1156030658614713</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B63">
+        <v>0.2058788810495588</v>
+      </c>
+      <c r="C63">
+        <v>0.134474776128396</v>
+      </c>
+      <c r="D63">
+        <v>0.2772829859707216</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B64">
+        <v>0.1986631874191323</v>
+      </c>
+      <c r="C64">
+        <v>0.1310071918645423</v>
+      </c>
+      <c r="D64">
+        <v>0.2663191829737223</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B65">
+        <v>0.2089163878490449</v>
+      </c>
+      <c r="C65">
+        <v>0.1974025289192148</v>
+      </c>
+      <c r="D65">
+        <v>0.2204302467788751</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B66">
         <v>0.2012906787155591</v>
       </c>
-      <c r="C50">
+      <c r="C66">
         <v>0.1905043980709452</v>
       </c>
-      <c r="D50">
+      <c r="D66">
         <v>0.212076959360173</v>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
         <is>
           <t>Preto ou pardo</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="G66" t="inlineStr">
         <is>
           <t>Rural</t>
         </is>

</xml_diff>

<commit_message>
Ajustes para acresentar linhas de totais
</commit_message>
<xml_diff>
--- a/outputs/mvp/ind_1_1_1/ind_1_1_1.xlsx
+++ b/outputs/mvp/ind_1_1_1/ind_1_1_1.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -459,18 +459,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.03836442158217402</v>
+        <v>0.04370877102601914</v>
       </c>
       <c r="C5">
-        <v>0.01923234229945393</v>
+        <v>0.02261369292706471</v>
       </c>
       <c r="D5">
-        <v>0.05749650086489411</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
+        <v>0.06480384912497357</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -485,22 +480,17 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.04922019959981231</v>
+        <v>0.05787220576945607</v>
       </c>
       <c r="C6">
-        <v>0.02047016498604594</v>
+        <v>0.05564693642397833</v>
       </c>
       <c r="D6">
-        <v>0.07797023421357868</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
+        <v>0.06009747511493381</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Branca</t>
         </is>
       </c>
     </row>
@@ -511,22 +501,17 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.05719558779292232</v>
+        <v>0.5997935013907915</v>
       </c>
       <c r="C7">
-        <v>0.0545962583504882</v>
+        <v>0.0273704173428474</v>
       </c>
       <c r="D7">
-        <v>0.05979491723535645</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
+        <v>1.172216585438735</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Ignorado</t>
         </is>
       </c>
     </row>
@@ -537,22 +522,17 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.05860772739432404</v>
+        <v>0.1873701569206996</v>
       </c>
       <c r="C8">
-        <v>0.05615703691342971</v>
+        <v>0.1340915401579178</v>
       </c>
       <c r="D8">
-        <v>0.06105841787521837</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
+        <v>0.2406487736834815</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Indígena</t>
         </is>
       </c>
     </row>
@@ -563,22 +543,17 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.547942177629459</v>
+        <v>0.1487959987401526</v>
       </c>
       <c r="C9">
-        <v>-0.05354854053967262</v>
+        <v>0.1450019350189764</v>
       </c>
       <c r="D9">
-        <v>1.14943289579859</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
+        <v>0.1525900624613288</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Ignorado</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
     </row>
@@ -589,22 +564,17 @@
         </is>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0.07787137915612806</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0.07517004345794608</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Ignorado</t>
+        <v>0.08057271485431004</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -615,22 +585,17 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.1690496088382455</v>
+        <v>0.275492340303849</v>
       </c>
       <c r="C11">
-        <v>0.112277010422408</v>
+        <v>0.2676700675264468</v>
       </c>
       <c r="D11">
-        <v>0.2258222072540829</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Indígena</t>
+        <v>0.2833146130812512</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Rural</t>
         </is>
       </c>
     </row>
@@ -641,22 +606,22 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.2056090128440956</v>
+        <v>0.03836442158217402</v>
       </c>
       <c r="C12">
-        <v>0.1412154026158309</v>
+        <v>0.01923234229945393</v>
       </c>
       <c r="D12">
-        <v>0.2700026230723603</v>
+        <v>0.05749650086489411</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Amarela</t>
         </is>
       </c>
     </row>
@@ -667,22 +632,22 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.1520285941557457</v>
+        <v>0.04922019959981231</v>
       </c>
       <c r="C13">
-        <v>0.1480190680868821</v>
+        <v>0.02047016498604594</v>
       </c>
       <c r="D13">
-        <v>0.1560381202246092</v>
+        <v>0.07797023421357868</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Amarela</t>
         </is>
       </c>
     </row>
@@ -693,22 +658,22 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.1455411125169712</v>
+        <v>0.05719558779292232</v>
       </c>
       <c r="C14">
-        <v>0.141489102453384</v>
+        <v>0.0545962583504882</v>
       </c>
       <c r="D14">
-        <v>0.1495931225805584</v>
+        <v>0.05979491723535645</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Branca</t>
         </is>
       </c>
     </row>
@@ -719,27 +684,22 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.03414687468430796</v>
+        <v>0.05860772739432404</v>
       </c>
       <c r="C15">
-        <v>0.01442365872164525</v>
+        <v>0.05615703691342971</v>
       </c>
       <c r="D15">
-        <v>0.05387009064697067</v>
+        <v>0.06105841787521837</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Amarela</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Branca</t>
         </is>
       </c>
     </row>
@@ -750,27 +710,22 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.0395175403864721</v>
+        <v>0.547942177629459</v>
       </c>
       <c r="C16">
-        <v>0.009159216176208244</v>
+        <v>-0.05354854053967262</v>
       </c>
       <c r="D16">
-        <v>0.06987586459673596</v>
+        <v>1.14943289579859</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Amarela</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Ignorado</t>
         </is>
       </c>
     </row>
@@ -781,27 +736,22 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.0429929756238225</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0.0402810519915398</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0.04570489925610521</v>
+        <v>1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Ignorado</t>
         </is>
       </c>
     </row>
@@ -812,27 +762,22 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.04361804634938695</v>
+        <v>0.1690496088382455</v>
       </c>
       <c r="C18">
-        <v>0.04104223264545248</v>
+        <v>0.112277010422408</v>
       </c>
       <c r="D18">
-        <v>0.04619386005332142</v>
+        <v>0.2258222072540829</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Indígena</t>
         </is>
       </c>
     </row>
@@ -843,27 +788,22 @@
         </is>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0.2056090128440956</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0.1412154026158309</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0.2700026230723603</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Ignorado</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Indígena</t>
         </is>
       </c>
     </row>
@@ -874,27 +814,22 @@
         </is>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0.1520285941557457</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0.1480190680868821</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0.1560381202246092</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Ignorado</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
     </row>
@@ -905,27 +840,22 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.1269812982491658</v>
+        <v>0.1455411125169712</v>
       </c>
       <c r="C21">
-        <v>0.06822599463120882</v>
+        <v>0.141489102453384</v>
       </c>
       <c r="D21">
-        <v>0.1857366018671228</v>
+        <v>0.1495931225805584</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Indígena</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
     </row>
@@ -936,22 +866,17 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.1681675975568784</v>
+        <v>0.07960486411426761</v>
       </c>
       <c r="C22">
-        <v>0.09693889576422837</v>
+        <v>0.07665994852757466</v>
       </c>
       <c r="D22">
-        <v>0.2393962993495284</v>
+        <v>0.08254977970096056</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Indígena</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -967,22 +892,17 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.1141770562689356</v>
+        <v>0.0760234141979618</v>
       </c>
       <c r="C23">
-        <v>0.1096386265718891</v>
+        <v>0.07328431820352875</v>
       </c>
       <c r="D23">
-        <v>0.1187154859659822</v>
+        <v>0.07876251019239484</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Feminino</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Preto ou pardo</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -998,27 +918,22 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.1044096138081008</v>
+        <v>0.2816454394129765</v>
       </c>
       <c r="C24">
-        <v>0.1000724231128585</v>
+        <v>0.2732052673432614</v>
       </c>
       <c r="D24">
-        <v>0.1087468045033431</v>
+        <v>0.2900856114826916</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Preto ou pardo</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
@@ -1029,22 +944,17 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.1217234321957831</v>
+        <v>0.2698486153876987</v>
       </c>
       <c r="C25">
-        <v>0.04817577606463851</v>
+        <v>0.2617985094899438</v>
       </c>
       <c r="D25">
-        <v>0.1952710883269278</v>
+        <v>0.2778987212854536</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Feminino</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Amarela</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1060,18 +970,13 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.2064841774806512</v>
+        <v>0.03677676916635386</v>
       </c>
       <c r="C26">
-        <v>0.08366085869726865</v>
+        <v>0.01482927261515115</v>
       </c>
       <c r="D26">
-        <v>0.3293074962640338</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
+        <v>0.05872426571755657</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1080,7 +985,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -1091,18 +996,13 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.1786886683493295</v>
+        <v>0.04328992001688426</v>
       </c>
       <c r="C27">
-        <v>0.166166435152406</v>
+        <v>0.04090610951614845</v>
       </c>
       <c r="D27">
-        <v>0.191210901546253</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
+        <v>0.04567373051762007</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1111,7 +1011,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -1122,27 +1022,22 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.1693578553493132</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>0.1585350259976693</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>0.1801806847009571</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
+        <v>1</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Ignorado</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -1153,27 +1048,22 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.3898343053661995</v>
+        <v>0.1476720238324589</v>
       </c>
       <c r="C29">
-        <v>-0.2954529790628765</v>
+        <v>0.09128142238012218</v>
       </c>
       <c r="D29">
-        <v>1.075121589795276</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
+        <v>0.2040626252847957</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Ignorado</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -1184,27 +1074,22 @@
         </is>
       </c>
       <c r="B30">
-        <v>0.3641963620849838</v>
+        <v>0.1093713682272884</v>
       </c>
       <c r="C30">
-        <v>0.2206456189526247</v>
+        <v>0.1051975352627313</v>
       </c>
       <c r="D30">
-        <v>0.507747105217343</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
+        <v>0.1135452011918455</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -1215,22 +1100,17 @@
         </is>
       </c>
       <c r="B31">
-        <v>0.3843262963645647</v>
+        <v>0.1674255666515624</v>
       </c>
       <c r="C31">
-        <v>0.2449107313705934</v>
+        <v>0.08273920921421367</v>
       </c>
       <c r="D31">
-        <v>0.5237418613585361</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
+        <v>0.2521119240889112</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Amarela</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1246,22 +1126,17 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.3367118684632939</v>
+        <v>0.1739144304880306</v>
       </c>
       <c r="C32">
-        <v>0.3268788949605854</v>
+        <v>0.1632529277464306</v>
       </c>
       <c r="D32">
-        <v>0.3465448419660024</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
+        <v>0.1845759332296306</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1277,22 +1152,17 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.3201489087125678</v>
+        <v>0.3898343053661995</v>
       </c>
       <c r="C33">
-        <v>0.3107084358507918</v>
+        <v>-0.2954529790628765</v>
       </c>
       <c r="D33">
-        <v>0.3295893815743438</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
+        <v>1.075121589795276</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Ignorado</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1304,339 +1174,414 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B34">
-        <v>0.06924122814792455</v>
+        <v>0.3741652421387036</v>
       </c>
       <c r="C34">
-        <v>0.06700591338730398</v>
+        <v>0.2404440189904349</v>
       </c>
       <c r="D34">
-        <v>0.07147654290854512</v>
+        <v>0.5078864652869721</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B35">
-        <v>0.06969957259703537</v>
+        <v>0.3279867463624598</v>
       </c>
       <c r="C35">
-        <v>0.06736003505919752</v>
+        <v>0.3188641701071479</v>
       </c>
       <c r="D35">
-        <v>0.07203911013487321</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Feminino</t>
+        <v>0.3371093226177717</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B36">
-        <v>0.06876192800282943</v>
+        <v>0.03414687468430796</v>
       </c>
       <c r="C36">
-        <v>0.06636935892646212</v>
+        <v>0.01442365872164525</v>
       </c>
       <c r="D36">
-        <v>0.07115449707919674</v>
+        <v>0.05387009064697067</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B37">
-        <v>0.05690056744754991</v>
+        <v>0.0395175403864721</v>
       </c>
       <c r="C37">
-        <v>0.04000406267686278</v>
+        <v>0.009159216176208244</v>
       </c>
       <c r="D37">
-        <v>0.07379707221823704</v>
+        <v>0.06987586459673596</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
           <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B38">
-        <v>0.0630473992577661</v>
+        <v>0.0429929756238225</v>
       </c>
       <c r="C38">
-        <v>0.03570223759902014</v>
+        <v>0.0402810519915398</v>
       </c>
       <c r="D38">
-        <v>0.09039256091651207</v>
+        <v>0.04570489925610521</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B39">
-        <v>0.040116023202247</v>
+        <v>0.04361804634938695</v>
       </c>
       <c r="C39">
-        <v>0.03789355035290268</v>
+        <v>0.04104223264545248</v>
       </c>
       <c r="D39">
-        <v>0.04233849605159132</v>
+        <v>0.04619386005332142</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
           <t>Branca</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B40">
-        <v>0.03952726715739519</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>0.03721841441200474</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>0.04183611990278564</v>
+        <v>1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B41">
-        <v>0.04397793649124208</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>-0.02727489791412698</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>0.1152307708966111</v>
+        <v>1</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
           <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B42">
-        <v>0.1288491536471042</v>
+        <v>0.1269812982491658</v>
       </c>
       <c r="C42">
-        <v>-0.04901483159892142</v>
+        <v>0.06822599463120882</v>
       </c>
       <c r="D42">
-        <v>0.3067131388931298</v>
+        <v>0.1857366018671228</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Ignorado</t>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B43">
-        <v>0.09077607592597677</v>
+        <v>0.1681675975568784</v>
       </c>
       <c r="C43">
-        <v>0.06614113963765586</v>
+        <v>0.09693889576422837</v>
       </c>
       <c r="D43">
-        <v>0.1154110122142977</v>
+        <v>0.2393962993495284</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
           <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B44">
-        <v>0.08603253087970009</v>
+        <v>0.1141770562689356</v>
       </c>
       <c r="C44">
-        <v>0.06052607930385365</v>
+        <v>0.1096386265718891</v>
       </c>
       <c r="D44">
-        <v>0.1115389824555465</v>
+        <v>0.1187154859659822</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B45">
-        <v>0.09289066147244007</v>
+        <v>0.1044096138081008</v>
       </c>
       <c r="C45">
-        <v>0.08933422823958206</v>
+        <v>0.1000724231128585</v>
       </c>
       <c r="D45">
-        <v>0.09644709470529808</v>
+        <v>0.1087468045033431</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
           <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B46">
-        <v>0.09052670600977686</v>
+        <v>0.1217234321957831</v>
       </c>
       <c r="C46">
-        <v>0.08722282219865291</v>
+        <v>0.04817577606463851</v>
       </c>
       <c r="D46">
-        <v>0.09383058982090081</v>
+        <v>0.1952710883269278</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B47">
-        <v>0.05337295832516659</v>
+        <v>0.2064841774806512</v>
       </c>
       <c r="C47">
-        <v>0.03519586192159806</v>
+        <v>0.08366085869726865</v>
       </c>
       <c r="D47">
-        <v>0.07155005472873513</v>
+        <v>0.3293074962640338</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1646,59 +1591,59 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B48">
-        <v>0.04906234186894141</v>
+        <v>0.1786886683493295</v>
       </c>
       <c r="C48">
-        <v>0.01906166929770911</v>
+        <v>0.166166435152406</v>
       </c>
       <c r="D48">
-        <v>0.0790630144401737</v>
+        <v>0.191210901546253</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Amarela</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B49">
-        <v>0.03247678207038816</v>
+        <v>0.1693578553493132</v>
       </c>
       <c r="C49">
-        <v>0.0302513465389829</v>
+        <v>0.1585350259976693</v>
       </c>
       <c r="D49">
-        <v>0.03470221760179343</v>
+        <v>0.1801806847009571</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1708,55 +1653,55 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B50">
-        <v>0.03104802298978394</v>
+        <v>0.3898343053661995</v>
       </c>
       <c r="C50">
-        <v>0.02876501123393008</v>
+        <v>-0.2954529790628765</v>
       </c>
       <c r="D50">
-        <v>0.03333103474563781</v>
+        <v>1.075121589795276</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Ignorado</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B51">
-        <v>0.04409003357927133</v>
+        <v>0.3641963620849838</v>
       </c>
       <c r="C51">
-        <v>-0.02740207776296817</v>
+        <v>0.2206456189526247</v>
       </c>
       <c r="D51">
-        <v>0.1155821449215108</v>
+        <v>0.507747105217343</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1765,29 +1710,29 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Ignorado</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B52">
-        <v>0.1309669316087286</v>
+        <v>0.3843262963645647</v>
       </c>
       <c r="C52">
-        <v>-0.04965823300381697</v>
+        <v>0.2449107313705934</v>
       </c>
       <c r="D52">
-        <v>0.3115920962212742</v>
+        <v>0.5237418613585361</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1796,29 +1741,29 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Ignorado</t>
+          <t>Indígena</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B53">
-        <v>0.07000629753765267</v>
+        <v>0.3367118684632939</v>
       </c>
       <c r="C53">
-        <v>0.04284481472592563</v>
+        <v>0.3268788949605854</v>
       </c>
       <c r="D53">
-        <v>0.0971677803493797</v>
+        <v>0.3465448419660024</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1827,29 +1772,29 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B54">
-        <v>0.05942416420103389</v>
+        <v>0.3201489087125678</v>
       </c>
       <c r="C54">
-        <v>0.03182497350489777</v>
+        <v>0.3107084358507918</v>
       </c>
       <c r="D54">
-        <v>0.08702335489717</v>
+        <v>0.3295893815743438</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1858,12 +1803,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Indígena</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Urbana</t>
+          <t>Rural</t>
         </is>
       </c>
     </row>
@@ -1874,28 +1819,13 @@
         </is>
       </c>
       <c r="B55">
-        <v>0.07286359808387763</v>
+        <v>0.06924122814792455</v>
       </c>
       <c r="C55">
-        <v>0.06942407948457623</v>
+        <v>0.06700591338730398</v>
       </c>
       <c r="D55">
-        <v>0.07630311668317903</v>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Preto ou pardo</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Urbana</t>
-        </is>
+        <v>0.07147654290854512</v>
       </c>
     </row>
     <row r="56">
@@ -1905,27 +1835,17 @@
         </is>
       </c>
       <c r="B56">
-        <v>0.06860137834941644</v>
+        <v>0.06969957259703537</v>
       </c>
       <c r="C56">
-        <v>0.06528994464618545</v>
+        <v>0.06736003505919752</v>
       </c>
       <c r="D56">
-        <v>0.07191281205264743</v>
+        <v>0.07203911013487321</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>Preto ou pardo</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>Urbana</t>
+          <t>Feminino</t>
         </is>
       </c>
     </row>
@@ -1936,27 +1856,17 @@
         </is>
       </c>
       <c r="B57">
-        <v>0.09380635946879537</v>
+        <v>0.06876192800282943</v>
       </c>
       <c r="C57">
-        <v>0.04549894925610921</v>
+        <v>0.06636935892646212</v>
       </c>
       <c r="D57">
-        <v>0.1421137696814815</v>
+        <v>0.07115449707919674</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Feminino</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Amarela</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Masculino</t>
         </is>
       </c>
     </row>
@@ -1967,27 +1877,17 @@
         </is>
       </c>
       <c r="B58">
-        <v>0.1739309196846933</v>
+        <v>0.05960598826985351</v>
       </c>
       <c r="C58">
-        <v>0.1188232112976242</v>
+        <v>0.04187632193071125</v>
       </c>
       <c r="D58">
-        <v>0.2290386280717624</v>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
+        <v>0.07733565460899576</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
           <t>Amarela</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Rural</t>
         </is>
       </c>
     </row>
@@ -1998,27 +1898,17 @@
         </is>
       </c>
       <c r="B59">
-        <v>0.1115463158419633</v>
+        <v>0.03983168975973562</v>
       </c>
       <c r="C59">
-        <v>0.1015179294887903</v>
+        <v>0.03781779824525358</v>
       </c>
       <c r="D59">
-        <v>0.1215747021951363</v>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
+        <v>0.04184558127421766</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
           <t>Branca</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>Rural</t>
         </is>
       </c>
     </row>
@@ -2029,27 +1919,17 @@
         </is>
       </c>
       <c r="B60">
-        <v>0.106629481332095</v>
+        <v>0.078409435207292</v>
       </c>
       <c r="C60">
-        <v>0.09765589680271874</v>
+        <v>-0.03685236837095079</v>
       </c>
       <c r="D60">
-        <v>0.1156030658614713</v>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
+        <v>0.1936712387855348</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Branca</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Ignorado</t>
         </is>
       </c>
     </row>
@@ -2060,27 +1940,17 @@
         </is>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>0.08859003541810076</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.06746605194460328</v>
       </c>
       <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
+        <v>0.1097140188915982</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Ignorado</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Indígena</t>
         </is>
       </c>
     </row>
@@ -2091,27 +1961,17 @@
         </is>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>0.09172212331250452</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>0.08851028794319181</v>
       </c>
       <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
+        <v>0.09493395868181724</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Ignorado</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Preto ou pardo</t>
         </is>
       </c>
     </row>
@@ -2122,27 +1982,17 @@
         </is>
       </c>
       <c r="B63">
-        <v>0.2058788810495588</v>
+        <v>0.05335293419066042</v>
       </c>
       <c r="C63">
-        <v>0.134474776128396</v>
+        <v>0.05118512566217364</v>
       </c>
       <c r="D63">
-        <v>0.2772829859707216</v>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>Indígena</t>
-        </is>
+        <v>0.0555207427191472</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Rural</t>
+          <t>Urbana</t>
         </is>
       </c>
     </row>
@@ -2153,23 +2003,13 @@
         </is>
       </c>
       <c r="B64">
-        <v>0.1986631874191323</v>
+        <v>0.1724438778041334</v>
       </c>
       <c r="C64">
-        <v>0.1310071918645423</v>
+        <v>0.1639628049029017</v>
       </c>
       <c r="D64">
-        <v>0.2663191829737223</v>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Indígena</t>
-        </is>
+        <v>0.1809249507053652</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2184,13 +2024,13 @@
         </is>
       </c>
       <c r="B65">
-        <v>0.2089163878490449</v>
+        <v>0.05690056744754991</v>
       </c>
       <c r="C65">
-        <v>0.1974025289192148</v>
+        <v>0.04000406267686278</v>
       </c>
       <c r="D65">
-        <v>0.2204302467788751</v>
+        <v>0.07379707221823704</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2199,12 +2039,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Preto ou pardo</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>Rural</t>
+          <t>Amarela</t>
         </is>
       </c>
     </row>
@@ -2215,25 +2050,1212 @@
         </is>
       </c>
       <c r="B66">
+        <v>0.0630473992577661</v>
+      </c>
+      <c r="C66">
+        <v>0.03570223759902014</v>
+      </c>
+      <c r="D66">
+        <v>0.09039256091651207</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Amarela</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B67">
+        <v>0.040116023202247</v>
+      </c>
+      <c r="C67">
+        <v>0.03789355035290268</v>
+      </c>
+      <c r="D67">
+        <v>0.04233849605159132</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B68">
+        <v>0.03952726715739519</v>
+      </c>
+      <c r="C68">
+        <v>0.03721841441200474</v>
+      </c>
+      <c r="D68">
+        <v>0.04183611990278564</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B69">
+        <v>0.04397793649124208</v>
+      </c>
+      <c r="C69">
+        <v>-0.02727489791412698</v>
+      </c>
+      <c r="D69">
+        <v>0.1152307708966111</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B70">
+        <v>0.1288491536471042</v>
+      </c>
+      <c r="C70">
+        <v>-0.04901483159892142</v>
+      </c>
+      <c r="D70">
+        <v>0.3067131388931298</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B71">
+        <v>0.09077607592597677</v>
+      </c>
+      <c r="C71">
+        <v>0.06614113963765586</v>
+      </c>
+      <c r="D71">
+        <v>0.1154110122142977</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B72">
+        <v>0.08603253087970009</v>
+      </c>
+      <c r="C72">
+        <v>0.06052607930385365</v>
+      </c>
+      <c r="D72">
+        <v>0.1115389824555465</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B73">
+        <v>0.09289066147244007</v>
+      </c>
+      <c r="C73">
+        <v>0.08933422823958206</v>
+      </c>
+      <c r="D73">
+        <v>0.09644709470529808</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B74">
+        <v>0.09052670600977686</v>
+      </c>
+      <c r="C74">
+        <v>0.08722282219865291</v>
+      </c>
+      <c r="D74">
+        <v>0.09383058982090081</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B75">
+        <v>0.05461545307270359</v>
+      </c>
+      <c r="C75">
+        <v>0.05235938007005467</v>
+      </c>
+      <c r="D75">
+        <v>0.0568715260753525</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B76">
+        <v>0.05200536719821165</v>
+      </c>
+      <c r="C76">
+        <v>0.04961384326208126</v>
+      </c>
+      <c r="D76">
+        <v>0.05439689113434205</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B77">
+        <v>0.1755424564568883</v>
+      </c>
+      <c r="C77">
+        <v>0.1665292239389371</v>
+      </c>
+      <c r="D77">
+        <v>0.1845556889748395</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B78">
+        <v>0.1696072384212494</v>
+      </c>
+      <c r="C78">
+        <v>0.1610121452809155</v>
+      </c>
+      <c r="D78">
+        <v>0.1782023315615833</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B79">
+        <v>0.05150486990196568</v>
+      </c>
+      <c r="C79">
+        <v>0.03224923615644512</v>
+      </c>
+      <c r="D79">
+        <v>0.07076050364748625</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B80">
+        <v>0.03179297985135296</v>
+      </c>
+      <c r="C80">
+        <v>0.02982897317791521</v>
+      </c>
+      <c r="D80">
+        <v>0.03375698652479071</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B81">
+        <v>0.07904744000443985</v>
+      </c>
+      <c r="C81">
+        <v>-0.03709074331815805</v>
+      </c>
+      <c r="D81">
+        <v>0.1951856233270378</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B82">
+        <v>0.065250768183631</v>
+      </c>
+      <c r="C82">
+        <v>0.04236858353087872</v>
+      </c>
+      <c r="D82">
+        <v>0.08813295283638328</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B83">
+        <v>0.07077949236208034</v>
+      </c>
+      <c r="C83">
+        <v>0.06766009368559568</v>
+      </c>
+      <c r="D83">
+        <v>0.07389889103856499</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B84">
+        <v>0.1340517109611397</v>
+      </c>
+      <c r="C84">
+        <v>0.0945146444299457</v>
+      </c>
+      <c r="D84">
+        <v>0.1735887774923336</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B85">
+        <v>0.1089881779048286</v>
+      </c>
+      <c r="C85">
+        <v>0.1002057928866261</v>
+      </c>
+      <c r="D85">
+        <v>0.117770562923031</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B87">
+        <v>0.2021514559654968</v>
+      </c>
+      <c r="C87">
+        <v>0.1438018808037381</v>
+      </c>
+      <c r="D87">
+        <v>0.2605010311272555</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B88">
+        <v>0.2049266508199169</v>
+      </c>
+      <c r="C88">
+        <v>0.1942795722943766</v>
+      </c>
+      <c r="D88">
+        <v>0.2155737293454573</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B89">
+        <v>0.05337295832516659</v>
+      </c>
+      <c r="C89">
+        <v>0.03519586192159806</v>
+      </c>
+      <c r="D89">
+        <v>0.07155005472873513</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B90">
+        <v>0.04906234186894141</v>
+      </c>
+      <c r="C90">
+        <v>0.01906166929770911</v>
+      </c>
+      <c r="D90">
+        <v>0.0790630144401737</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B91">
+        <v>0.03247678207038816</v>
+      </c>
+      <c r="C91">
+        <v>0.0302513465389829</v>
+      </c>
+      <c r="D91">
+        <v>0.03470221760179343</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B92">
+        <v>0.03104802298978394</v>
+      </c>
+      <c r="C92">
+        <v>0.02876501123393008</v>
+      </c>
+      <c r="D92">
+        <v>0.03333103474563781</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B93">
+        <v>0.04409003357927133</v>
+      </c>
+      <c r="C93">
+        <v>-0.02740207776296817</v>
+      </c>
+      <c r="D93">
+        <v>0.1155821449215108</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B94">
+        <v>0.1309669316087286</v>
+      </c>
+      <c r="C94">
+        <v>-0.04965823300381697</v>
+      </c>
+      <c r="D94">
+        <v>0.3115920962212742</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B95">
+        <v>0.07000629753765267</v>
+      </c>
+      <c r="C95">
+        <v>0.04284481472592563</v>
+      </c>
+      <c r="D95">
+        <v>0.0971677803493797</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B96">
+        <v>0.05942416420103389</v>
+      </c>
+      <c r="C96">
+        <v>0.03182497350489777</v>
+      </c>
+      <c r="D96">
+        <v>0.08702335489717</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B97">
+        <v>0.07286359808387763</v>
+      </c>
+      <c r="C97">
+        <v>0.06942407948457623</v>
+      </c>
+      <c r="D97">
+        <v>0.07630311668317903</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B98">
+        <v>0.06860137834941644</v>
+      </c>
+      <c r="C98">
+        <v>0.06528994464618545</v>
+      </c>
+      <c r="D98">
+        <v>0.07191281205264743</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B99">
+        <v>0.09380635946879537</v>
+      </c>
+      <c r="C99">
+        <v>0.04549894925610921</v>
+      </c>
+      <c r="D99">
+        <v>0.1421137696814815</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B100">
+        <v>0.1739309196846933</v>
+      </c>
+      <c r="C100">
+        <v>0.1188232112976242</v>
+      </c>
+      <c r="D100">
+        <v>0.2290386280717624</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Amarela</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B101">
+        <v>0.1115463158419633</v>
+      </c>
+      <c r="C101">
+        <v>0.1015179294887903</v>
+      </c>
+      <c r="D101">
+        <v>0.1215747021951363</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B102">
+        <v>0.106629481332095</v>
+      </c>
+      <c r="C102">
+        <v>0.09765589680271874</v>
+      </c>
+      <c r="D102">
+        <v>0.1156030658614713</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Ignorado</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B105">
+        <v>0.2058788810495588</v>
+      </c>
+      <c r="C105">
+        <v>0.134474776128396</v>
+      </c>
+      <c r="D105">
+        <v>0.2772829859707216</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B106">
+        <v>0.1986631874191323</v>
+      </c>
+      <c r="C106">
+        <v>0.1310071918645423</v>
+      </c>
+      <c r="D106">
+        <v>0.2663191829737223</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Indígena</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B107">
+        <v>0.2089163878490449</v>
+      </c>
+      <c r="C107">
+        <v>0.1974025289192148</v>
+      </c>
+      <c r="D107">
+        <v>0.2204302467788751</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Preto ou pardo</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B108">
         <v>0.2012906787155591</v>
       </c>
-      <c r="C66">
+      <c r="C108">
         <v>0.1905043980709452</v>
       </c>
-      <c r="D66">
+      <c r="D108">
         <v>0.212076959360173</v>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
         <is>
           <t>Preto ou pardo</t>
         </is>
       </c>
-      <c r="G66" t="inlineStr">
+      <c r="G108" t="inlineStr">
         <is>
           <t>Rural</t>
         </is>

</xml_diff>